<commit_message>
update trip 3 data
</commit_message>
<xml_diff>
--- a/data/taggingData/bycatchData.xlsx
+++ b/data/taggingData/bycatchData.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\chinTagging\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28280" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="124">
   <si>
     <t>set</t>
   </si>
@@ -238,16 +236,191 @@
   </si>
   <si>
     <t>vermillion rockfish</t>
+  </si>
+  <si>
+    <t>078</t>
+  </si>
+  <si>
+    <t>079</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>083</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>085</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>canary</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>089</t>
+  </si>
+  <si>
+    <t>090</t>
+  </si>
+  <si>
+    <t>091</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>095</t>
+  </si>
+  <si>
+    <t>096</t>
+  </si>
+  <si>
+    <t>097</t>
+  </si>
+  <si>
+    <t>098</t>
+  </si>
+  <si>
+    <t>099</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>sockeye</t>
+  </si>
+  <si>
+    <t>133</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,14 +443,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="39">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,7 +585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -371,7 +620,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -548,7 +797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,21 +805,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="L101" sqref="L101"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B216" sqref="B216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -584,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="str">
         <f>"CT2019"&amp;"_"&amp;B2</f>
         <v>CT2019_006</v>
@@ -599,7 +848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">"CT2019"&amp;"_"&amp;B3</f>
         <v>CT2019_007</v>
@@ -614,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_007</v>
@@ -629,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_008</v>
@@ -644,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_016</v>
@@ -659,7 +908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_017</v>
@@ -674,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_017</v>
@@ -689,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_018</v>
@@ -704,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_020</v>
@@ -719,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_021</v>
@@ -734,7 +983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_021</v>
@@ -749,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_022</v>
@@ -764,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_022</v>
@@ -779,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_023</v>
@@ -794,7 +1043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_023</v>
@@ -809,7 +1058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_024</v>
@@ -824,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_024</v>
@@ -839,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_025</v>
@@ -854,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_025</v>
@@ -869,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_026</v>
@@ -884,7 +1133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_026</v>
@@ -899,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_027</v>
@@ -914,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_029</v>
@@ -929,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_029</v>
@@ -944,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_031</v>
@@ -959,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_033</v>
@@ -974,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_033</v>
@@ -989,7 +1238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_034</v>
@@ -1004,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_034</v>
@@ -1019,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_034</v>
@@ -1034,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_035</v>
@@ -1049,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_036</v>
@@ -1064,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_037</v>
@@ -1079,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_037</v>
@@ -1094,7 +1343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_037</v>
@@ -1109,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_038</v>
@@ -1124,7 +1373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_038</v>
@@ -1139,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_038</v>
@@ -1154,7 +1403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_039</v>
@@ -1169,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_039</v>
@@ -1184,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_039</v>
@@ -1199,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_040</v>
@@ -1214,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_040</v>
@@ -1229,7 +1478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_041</v>
@@ -1244,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_041</v>
@@ -1259,7 +1508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_041</v>
@@ -1274,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_042</v>
@@ -1289,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_043</v>
@@ -1304,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_043</v>
@@ -1319,7 +1568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_043</v>
@@ -1334,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_044</v>
@@ -1349,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_044</v>
@@ -1364,7 +1613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_045</v>
@@ -1379,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_045</v>
@@ -1394,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_046</v>
@@ -1409,7 +1658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_047</v>
@@ -1424,7 +1673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_047</v>
@@ -1439,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_047</v>
@@ -1454,7 +1703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_048</v>
@@ -1469,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_048</v>
@@ -1484,7 +1733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_049</v>
@@ -1499,7 +1748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_049</v>
@@ -1514,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_050</v>
@@ -1529,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_050</v>
@@ -1544,7 +1793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_050</v>
@@ -1559,9 +1808,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" t="str">
-        <f t="shared" ref="A67:A102" si="1">"CT2019"&amp;"_"&amp;B67</f>
+        <f t="shared" ref="A67:A130" si="1">"CT2019"&amp;"_"&amp;B67</f>
         <v>CT2019_051</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1574,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_052</v>
@@ -1589,7 +1838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_053</v>
@@ -1604,7 +1853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_053</v>
@@ -1619,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_054</v>
@@ -1634,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_056</v>
@@ -1649,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_059</v>
@@ -1664,7 +1913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_060</v>
@@ -1679,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_060</v>
@@ -1694,7 +1943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_060</v>
@@ -1709,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_061</v>
@@ -1724,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_061</v>
@@ -1739,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_063</v>
@@ -1754,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_063</v>
@@ -1769,7 +2018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_064</v>
@@ -1784,7 +2033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_065</v>
@@ -1799,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_066</v>
@@ -1814,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_066</v>
@@ -1829,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_067</v>
@@ -1844,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_067</v>
@@ -1859,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_069</v>
@@ -1874,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_069</v>
@@ -1889,7 +2138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_070</v>
@@ -1904,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4">
       <c r="A90" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_070</v>
@@ -1919,7 +2168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4">
       <c r="A91" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_071</v>
@@ -1934,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4">
       <c r="A92" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_073</v>
@@ -1949,7 +2198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4">
       <c r="A93" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_073</v>
@@ -1964,7 +2213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4">
       <c r="A94" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_073</v>
@@ -1979,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4">
       <c r="A95" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_074</v>
@@ -1994,7 +2243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4">
       <c r="A96" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_075</v>
@@ -2009,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_076</v>
@@ -2024,7 +2273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_076</v>
@@ -2039,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4">
       <c r="A99" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_077</v>
@@ -2054,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4">
       <c r="A100" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_077</v>
@@ -2069,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4">
       <c r="A101" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_077</v>
@@ -2084,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4">
       <c r="A102" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_077</v>
@@ -2099,8 +2348,1709 @@
         <v>1</v>
       </c>
     </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_078</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_078</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C104" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_079</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_080</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
+        <v>17</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_080</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_081</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C108" t="s">
+        <v>17</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_081</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C109" t="s">
+        <v>34</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_081</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_082</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C111" t="s">
+        <v>34</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_082</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_083</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_084</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_084</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C115" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_085</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C116" t="s">
+        <v>32</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_085</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C117" t="s">
+        <v>40</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_086</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_086</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_087</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_087</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_087</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C122" t="s">
+        <v>40</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_088</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_089</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C124" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_090</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C125" t="s">
+        <v>17</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_091</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_091</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C127" t="s">
+        <v>34</v>
+      </c>
+      <c r="D127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_092</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C128" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_092</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C129" t="s">
+        <v>34</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="str">
+        <f t="shared" si="1"/>
+        <v>CT2019_092</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="str">
+        <f t="shared" ref="A131:A185" si="2">"CT2019"&amp;"_"&amp;B131</f>
+        <v>CT2019_095</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_096</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C132" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_096</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" t="s">
+        <v>34</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_096</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_097</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C135" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_097</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_098</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C137" t="s">
+        <v>17</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_098</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C138" t="s">
+        <v>34</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_099</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C139" t="s">
+        <v>17</v>
+      </c>
+      <c r="D139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_099</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C140" t="s">
+        <v>34</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_099</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C141" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_100</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C142" t="s">
+        <v>17</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_100</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C143" t="s">
+        <v>34</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_100</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C144" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_101</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C145" t="s">
+        <v>17</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_103</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C146" t="s">
+        <v>17</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_103</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C147" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_103</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_104</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C149" t="s">
+        <v>17</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_104</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C150" t="s">
+        <v>34</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_104</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C151" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_105</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C152" t="s">
+        <v>34</v>
+      </c>
+      <c r="D152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_105</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C153" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_106</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C154" t="s">
+        <v>34</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_106</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C155" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_107</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C156" t="s">
+        <v>34</v>
+      </c>
+      <c r="D156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_107</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C157" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_107</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_108</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C159" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_108</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C160" t="s">
+        <v>34</v>
+      </c>
+      <c r="D160">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_108</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C161" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_109</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C162" t="s">
+        <v>34</v>
+      </c>
+      <c r="D162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_109</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C163" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_110</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C164" t="s">
+        <v>34</v>
+      </c>
+      <c r="D164">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_110</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C165" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_111</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C166" t="s">
+        <v>34</v>
+      </c>
+      <c r="D166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_111</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C167" t="s">
+        <v>17</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_112</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C168" t="s">
+        <v>34</v>
+      </c>
+      <c r="D168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_113</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C169" t="s">
+        <v>17</v>
+      </c>
+      <c r="D169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_113</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_113</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C171" t="s">
+        <v>34</v>
+      </c>
+      <c r="D171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_114</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_114</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C173" t="s">
+        <v>34</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_114</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C174" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_116</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C175" t="s">
+        <v>17</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_116</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C176" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_116</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C177" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_116</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C178" t="s">
+        <v>34</v>
+      </c>
+      <c r="D178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_116</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C179" t="s">
+        <v>81</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_117</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C180" t="s">
+        <v>17</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_117</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C181" t="s">
+        <v>34</v>
+      </c>
+      <c r="D181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_117</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C182" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_118</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C183" t="s">
+        <v>17</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_119</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C184" t="s">
+        <v>17</v>
+      </c>
+      <c r="D184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="str">
+        <f t="shared" si="2"/>
+        <v>CT2019_119</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C185" t="s">
+        <v>34</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="str">
+        <f t="shared" ref="A186:A197" si="3">"CT2019"&amp;"_"&amp;B186</f>
+        <v>CT2019_119</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C186" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_119</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C187" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_120</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C188" t="s">
+        <v>17</v>
+      </c>
+      <c r="D188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_120</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C189" t="s">
+        <v>7</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_121</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C190" t="s">
+        <v>17</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_122</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C191" t="s">
+        <v>17</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_123</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C192" t="s">
+        <v>7</v>
+      </c>
+      <c r="D192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_124</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C193" t="s">
+        <v>17</v>
+      </c>
+      <c r="D193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_124</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C194" t="s">
+        <v>34</v>
+      </c>
+      <c r="D194">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_124</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C195" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_125</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C196" t="s">
+        <v>17</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_125</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C197" t="s">
+        <v>7</v>
+      </c>
+      <c r="D197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="str">
+        <f t="shared" ref="A198:A199" si="4">"CT2019"&amp;"_"&amp;B198</f>
+        <v>CT2019_125</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C198" t="s">
+        <v>34</v>
+      </c>
+      <c r="D198">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="str">
+        <f t="shared" si="4"/>
+        <v>CT2019_126</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="str">
+        <f t="shared" ref="A200:A215" si="5">"CT2019"&amp;"_"&amp;B200</f>
+        <v>CT2019_126</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C200" t="s">
+        <v>13</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_126</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C201" t="s">
+        <v>34</v>
+      </c>
+      <c r="D201">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_127</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C202" t="s">
+        <v>34</v>
+      </c>
+      <c r="D202">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_127</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C203" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_128</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C204" t="s">
+        <v>34</v>
+      </c>
+      <c r="D204">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_128</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C205" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_129</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C206" t="s">
+        <v>34</v>
+      </c>
+      <c r="D206">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_129</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C207" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_130</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C208" t="s">
+        <v>7</v>
+      </c>
+      <c r="D208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_130</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C209" t="s">
+        <v>34</v>
+      </c>
+      <c r="D209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_132</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C210" t="s">
+        <v>17</v>
+      </c>
+      <c r="D210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_132</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C211" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_132</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C212" t="s">
+        <v>122</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_132</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C213" t="s">
+        <v>34</v>
+      </c>
+      <c r="D213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_133</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C214" t="s">
+        <v>17</v>
+      </c>
+      <c r="D214">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_133</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C215" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2112,24 +4062,29 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update trip 4 data pt. 1
</commit_message>
<xml_diff>
--- a/data/taggingData/bycatchData.xlsx
+++ b/data/taggingData/bycatchData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="174">
   <si>
     <t>set</t>
   </si>
@@ -395,6 +395,156 @@
   </si>
   <si>
     <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>ling cod</t>
+  </si>
+  <si>
+    <t>sanddab</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>186</t>
   </si>
 </sst>
 </file>
@@ -443,8 +593,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -488,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -508,6 +696,25 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +734,25 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -805,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D215"/>
+  <dimension ref="A1:D294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C270" sqref="C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3805,7 +4031,7 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="str">
-        <f t="shared" ref="A200:A215" si="5">"CT2019"&amp;"_"&amp;B200</f>
+        <f t="shared" ref="A200:A242" si="5">"CT2019"&amp;"_"&amp;B200</f>
         <v>CT2019_126</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -4041,6 +4267,1191 @@
       </c>
       <c r="D215">
         <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_134</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C216" t="s">
+        <v>7</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_134</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C217" t="s">
+        <v>40</v>
+      </c>
+      <c r="D217">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_134</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C218" t="s">
+        <v>32</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_135</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C219" t="s">
+        <v>13</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_135</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C220" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_136</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C221" t="s">
+        <v>40</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_136</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C222" t="s">
+        <v>32</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_136</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C223" t="s">
+        <v>7</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_137</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C224" t="s">
+        <v>6</v>
+      </c>
+      <c r="D224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_137</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C225" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_138</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C226" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_139</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C227" t="s">
+        <v>7</v>
+      </c>
+      <c r="D227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_140</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C228" t="s">
+        <v>17</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_141</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C229" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_142</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C230" t="s">
+        <v>34</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_144</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C231" t="s">
+        <v>7</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_145</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C232" t="s">
+        <v>7</v>
+      </c>
+      <c r="D232">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_146</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C233" t="s">
+        <v>7</v>
+      </c>
+      <c r="D233">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_147</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C234" t="s">
+        <v>7</v>
+      </c>
+      <c r="D234">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_147</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C235" t="s">
+        <v>34</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_148</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C236" t="s">
+        <v>34</v>
+      </c>
+      <c r="D236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_148</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C237" t="s">
+        <v>7</v>
+      </c>
+      <c r="D237">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_149</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C238" t="s">
+        <v>7</v>
+      </c>
+      <c r="D238">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_149</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C239" t="s">
+        <v>34</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_149</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C240" t="s">
+        <v>17</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_150</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C241" t="s">
+        <v>7</v>
+      </c>
+      <c r="D241">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" t="str">
+        <f t="shared" si="5"/>
+        <v>CT2019_150</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C242" t="s">
+        <v>34</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" t="str">
+        <f t="shared" ref="A243:A294" si="6">"CT2019"&amp;"_"&amp;B243</f>
+        <v>CT2019_150</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C243" t="s">
+        <v>17</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_151</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C244" t="s">
+        <v>7</v>
+      </c>
+      <c r="D244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_152</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C245" t="s">
+        <v>17</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_152</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C246" t="s">
+        <v>34</v>
+      </c>
+      <c r="D246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_153</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C247" t="s">
+        <v>34</v>
+      </c>
+      <c r="D247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_153</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C248" t="s">
+        <v>7</v>
+      </c>
+      <c r="D248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_153</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C249" t="s">
+        <v>143</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_153</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C250" t="s">
+        <v>144</v>
+      </c>
+      <c r="D250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_154</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C251" t="s">
+        <v>7</v>
+      </c>
+      <c r="D251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_155</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C252" t="s">
+        <v>7</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_156</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C253" t="s">
+        <v>34</v>
+      </c>
+      <c r="D253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_158</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C254" t="s">
+        <v>17</v>
+      </c>
+      <c r="D254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_158</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C255" t="s">
+        <v>40</v>
+      </c>
+      <c r="D255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_158</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C256" t="s">
+        <v>7</v>
+      </c>
+      <c r="D256">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_159</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C257" t="s">
+        <v>7</v>
+      </c>
+      <c r="D257">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_159</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C258" t="s">
+        <v>34</v>
+      </c>
+      <c r="D258">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_160</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C259" t="s">
+        <v>7</v>
+      </c>
+      <c r="D259">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_161</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C260" t="s">
+        <v>17</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_161</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C261" t="s">
+        <v>7</v>
+      </c>
+      <c r="D261">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_162</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C262" t="s">
+        <v>7</v>
+      </c>
+      <c r="D262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_163</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C263" t="s">
+        <v>7</v>
+      </c>
+      <c r="D263">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_164</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C264" t="s">
+        <v>7</v>
+      </c>
+      <c r="D264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_166</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C265" t="s">
+        <v>34</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_167</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C266" t="s">
+        <v>7</v>
+      </c>
+      <c r="D266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_168</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C267" t="s">
+        <v>7</v>
+      </c>
+      <c r="D267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_170</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C268" t="s">
+        <v>17</v>
+      </c>
+      <c r="D268">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_170</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C269" t="s">
+        <v>7</v>
+      </c>
+      <c r="D269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
+      <c r="A270" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_171</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C270" t="s">
+        <v>17</v>
+      </c>
+      <c r="D270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
+      <c r="A271" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_171</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C271" t="s">
+        <v>7</v>
+      </c>
+      <c r="D271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
+      <c r="A272" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_172</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C272" t="s">
+        <v>7</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4">
+      <c r="A273" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_173</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C273" t="s">
+        <v>17</v>
+      </c>
+      <c r="D273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
+      <c r="A274" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_173</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C274" t="s">
+        <v>34</v>
+      </c>
+      <c r="D274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_173</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C275" t="s">
+        <v>7</v>
+      </c>
+      <c r="D275">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_174</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C276" t="s">
+        <v>17</v>
+      </c>
+      <c r="D276">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
+      <c r="A277" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_174</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C277" t="s">
+        <v>7</v>
+      </c>
+      <c r="D277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
+      <c r="A278" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_175</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C278" t="s">
+        <v>17</v>
+      </c>
+      <c r="D278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
+      <c r="A279" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_175</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C279" t="s">
+        <v>7</v>
+      </c>
+      <c r="D279">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_176</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C280" t="s">
+        <v>17</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_176</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C281" t="s">
+        <v>7</v>
+      </c>
+      <c r="D281">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_177</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C282" t="s">
+        <v>7</v>
+      </c>
+      <c r="D282">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_178</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C283" t="s">
+        <v>17</v>
+      </c>
+      <c r="D283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_178</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C284" t="s">
+        <v>7</v>
+      </c>
+      <c r="D284">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_179</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C285" t="s">
+        <v>17</v>
+      </c>
+      <c r="D285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_180</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C286" t="s">
+        <v>7</v>
+      </c>
+      <c r="D286">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_182</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C287" t="s">
+        <v>7</v>
+      </c>
+      <c r="D287">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_183</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C288" t="s">
+        <v>17</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_183</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C289" t="s">
+        <v>7</v>
+      </c>
+      <c r="D289">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_184</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C290" t="s">
+        <v>7</v>
+      </c>
+      <c r="D290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_185</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C291" t="s">
+        <v>17</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
+      <c r="A292" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_185</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C292" t="s">
+        <v>7</v>
+      </c>
+      <c r="D292">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_186</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C293" t="s">
+        <v>17</v>
+      </c>
+      <c r="D293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="A294" t="str">
+        <f t="shared" si="6"/>
+        <v>CT2019_186</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C294" t="s">
+        <v>34</v>
+      </c>
+      <c r="D294">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>